<commit_message>
Started adding mission data
</commit_message>
<xml_diff>
--- a/RKLB/RKLB.xlsx
+++ b/RKLB/RKLB.xlsx
@@ -5,21 +5,22 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/534a1defcf7f9d1a/Company Models CloudSave/RKLB/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Company-Models\RKLB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2533" documentId="8_{68811377-D074-4751-B59C-3812699B514B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5C2F2EDA-90B8-498B-B4E8-6799F7E276B2}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F916D81F-13A3-4FA1-9DFF-197BDCCCA38D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19110" yWindow="370" windowWidth="19200" windowHeight="10310" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="7" r:id="rId1"/>
     <sheet name="Info" sheetId="6" r:id="rId2"/>
     <sheet name="Model" sheetId="5" r:id="rId3"/>
-    <sheet name="Summary" sheetId="1" r:id="rId4"/>
-    <sheet name="Income Statement" sheetId="2" r:id="rId5"/>
-    <sheet name="Balance Sheet" sheetId="3" r:id="rId6"/>
-    <sheet name="Cash Flow" sheetId="4" r:id="rId7"/>
+    <sheet name="Missions" sheetId="8" r:id="rId4"/>
+    <sheet name="Summary" sheetId="1" r:id="rId5"/>
+    <sheet name="Income Statement" sheetId="2" r:id="rId6"/>
+    <sheet name="Balance Sheet" sheetId="3" r:id="rId7"/>
+    <sheet name="Cash Flow" sheetId="4" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -260,7 +261,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="909" uniqueCount="426">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1116" uniqueCount="445">
   <si>
     <t>Revenue per share</t>
   </si>
@@ -1730,6 +1731,63 @@
   </si>
   <si>
     <t xml:space="preserve">NASA's ELaNa-19 mission included the launch of many nano-satellites. </t>
+  </si>
+  <si>
+    <t>Missions</t>
+  </si>
+  <si>
+    <t>Sources</t>
+  </si>
+  <si>
+    <t>LEO, 500 km</t>
+  </si>
+  <si>
+    <t>RocketLab</t>
+  </si>
+  <si>
+    <t>Flight Test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LEO   </t>
+  </si>
+  <si>
+    <t>"Its's a Test"</t>
+  </si>
+  <si>
+    <t>"Two Thumbs Up"</t>
+  </si>
+  <si>
+    <t>DARPA</t>
+  </si>
+  <si>
+    <t>"That's a Funny Looking Cactus"</t>
+  </si>
+  <si>
+    <t>R3D2:DARPA</t>
+  </si>
+  <si>
+    <t>SPARC-1:US Air Force, Falcon ODE:US Air Force, Harbringer:US Air Force</t>
+  </si>
+  <si>
+    <t>LEO, 425 km, 39.5 deg</t>
+  </si>
+  <si>
+    <t>LEO, 500 km, 40 deg</t>
+  </si>
+  <si>
+    <t>Payload Mass (kg)</t>
+  </si>
+  <si>
+    <t>US Air Force</t>
+  </si>
+  <si>
+    <t>"Make it Rain</t>
+  </si>
+  <si>
+    <t>LEO</t>
+  </si>
+  <si>
+    <t>BlackSky Global 3:BlackSky, Prometheus:USSOCOM</t>
   </si>
 </sst>
 </file>
@@ -1998,7 +2056,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -2072,6 +2130,22 @@
     <xf numFmtId="14" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2088,10 +2162,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2218,9 +2288,7 @@
     <v>3.48</v>
     <v>1.8839999999999999</v>
     <v>-0.17</v>
-    <v>-2.5575000000000001E-2</v>
     <v>-4.1666999999999996E-2</v>
-    <v>-0.1</v>
     <v>USD</v>
     <v>Rocket Lab USA, Inc. is an end-to-end space company. The Company designs and manufactures small and medium-class rockets, spacecraft and spacecraft components to support the space economy. The Company delivers reliable launch services, spacecraft design services, spacecraft components, spacecraft manufacturing, and other spacecraft and on-orbit management solutions that make it easier to access space. It operates through two segments: Launch Services and Space Systems. Its Launch Services segment provides launch services to customers on a dedicated mission or ride share basis. Its Space Systems segment is comprised of space engineering, program management, spacecraft components, spacecraft manufacturing and mission operations. Its spacecraft component solutions are used to build spacecrafts, which include reaction wheels, star trackers, magnetic torque rods, solar panels, radios, separation systems, command and control spacecraft software, separation systems, and power solutions.</v>
     <v>1400</v>
@@ -2240,11 +2308,10 @@
     <v>4.05</v>
     <v>4.08</v>
     <v>3.91</v>
-    <v>3.81</v>
     <v>477649300</v>
     <v>RKLB</v>
     <v>ROCKET LAB USA, INC. (XNAS:RKLB)</v>
-    <v>6357609</v>
+    <v>5003</v>
     <v>3814888</v>
     <v>2021</v>
   </rv>
@@ -2276,9 +2343,7 @@
     <k n="52 week low"/>
     <k n="Beta"/>
     <k n="Change"/>
-    <k n="Change % (Extended hours)"/>
     <k n="Change (%)"/>
-    <k n="Change (Extended hours)"/>
     <k n="Currency" t="s"/>
     <k n="Description" t="s"/>
     <k n="Employees"/>
@@ -2298,7 +2363,6 @@
     <k n="Open"/>
     <k n="Previous close"/>
     <k n="Price"/>
-    <k n="Price (Extended hours)"/>
     <k n="Shares outstanding"/>
     <k n="Ticker symbol" t="s"/>
     <k n="UniqueName" t="s"/>
@@ -2315,7 +2379,7 @@
 <file path=xl/richData/rdsupportingpropertybag.xml><?xml version="1.0" encoding="utf-8"?>
 <supportingPropertyBags xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2">
   <spbArrays count="1">
-    <a count="44">
+    <a count="41">
       <v t="s">%EntityServiceId</v>
       <v t="s">_Format</v>
       <v t="s">%IsRefreshable</v>
@@ -2326,16 +2390,13 @@
       <v t="s">Name</v>
       <v t="s">_SubLabel</v>
       <v t="s">Price</v>
-      <v t="s">Price (Extended hours)</v>
       <v t="s">Exchange</v>
       <v t="s">Official name</v>
       <v t="s">Last trade time</v>
       <v t="s">Ticker symbol</v>
       <v t="s">Exchange abbreviation</v>
       <v t="s">Change</v>
-      <v t="s">Change (Extended hours)</v>
       <v t="s">Change (%)</v>
-      <v t="s">Change % (Extended hours)</v>
       <v t="s">Currency</v>
       <v t="s">Previous close</v>
       <v t="s">Open</v>
@@ -2399,19 +2460,13 @@
       <v>8</v>
       <v>9</v>
       <v>4</v>
-      <v>1</v>
-      <v>1</v>
-      <v>5</v>
     </spb>
     <spb s="4">
-      <v>at close</v>
+      <v>Real-Time Nasdaq Last Sale</v>
       <v>from previous close</v>
       <v>from previous close</v>
       <v>Source: Nasdaq Last Sale</v>
       <v>GMT</v>
-      <v>Real-Time Nasdaq Last Sale</v>
-      <v>from close</v>
-      <v>from close</v>
     </spb>
   </spbData>
 </supportingPropertyBags>
@@ -2455,9 +2510,6 @@
     <k n="Year incorporated" t="i"/>
     <k n="`%EntityServiceId" t="i"/>
     <k n="Shares outstanding" t="i"/>
-    <k n="Price (Extended hours)" t="i"/>
-    <k n="Change (Extended hours)" t="i"/>
-    <k n="Change % (Extended hours)" t="i"/>
   </s>
   <s>
     <k n="Price" t="s"/>
@@ -2465,9 +2517,6 @@
     <k n="Change (%)" t="s"/>
     <k n="ExchangeID" t="s"/>
     <k n="Last trade time" t="s"/>
-    <k n="Price (Extended hours)" t="s"/>
-    <k n="Change (Extended hours)" t="s"/>
-    <k n="Change % (Extended hours)" t="s"/>
   </s>
 </spbStructures>
 </file>
@@ -2939,8 +2988,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCD30AF4-E88D-45C6-BD68-9606C269A01E}">
   <dimension ref="A4:M130"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C52" sqref="C52"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -11702,6 +11751,1089 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AEFB4E4-DCFC-493A-A757-067ACB0ACC13}">
+  <dimension ref="A1:P139"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="C31" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="C82" sqref="C82"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="18.453125" customWidth="1"/>
+    <col min="3" max="3" width="10.453125" style="66" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A1" s="65" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="E2" s="5">
+        <v>43450</v>
+      </c>
+      <c r="F2" s="70">
+        <v>0.27291666666666664</v>
+      </c>
+      <c r="G2" t="s">
+        <v>342</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>419</v>
+      </c>
+      <c r="I2" t="s">
+        <v>422</v>
+      </c>
+      <c r="J2">
+        <v>78</v>
+      </c>
+      <c r="K2" t="s">
+        <v>408</v>
+      </c>
+      <c r="L2" t="s">
+        <v>414</v>
+      </c>
+      <c r="M2" t="b">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2" t="s">
+        <v>423</v>
+      </c>
+      <c r="P2" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="6" t="s">
+        <v>426</v>
+      </c>
+      <c r="C4" s="67"/>
+    </row>
+    <row r="5" spans="1:16" s="30" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="30" t="s">
+        <v>432</v>
+      </c>
+      <c r="C5" s="68"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
+        <v>398</v>
+      </c>
+      <c r="C6" s="69">
+        <v>42882</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="B7" t="s">
+        <v>397</v>
+      </c>
+      <c r="C7" s="70">
+        <v>0.18055555555555555</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="B8" t="s">
+        <v>399</v>
+      </c>
+      <c r="C8" s="66" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="B9" t="s">
+        <v>385</v>
+      </c>
+      <c r="C9" s="66" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="B10" t="s">
+        <v>400</v>
+      </c>
+      <c r="C10" s="66" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="B11" t="s">
+        <v>440</v>
+      </c>
+      <c r="C11" s="66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="B12" t="s">
+        <v>402</v>
+      </c>
+      <c r="C12" s="66" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="B13" t="s">
+        <v>404</v>
+      </c>
+      <c r="C13" s="66" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="B14" t="s">
+        <v>405</v>
+      </c>
+      <c r="C14" s="66" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="B15" t="s">
+        <v>403</v>
+      </c>
+      <c r="C15" s="66" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="B16" t="s">
+        <v>424</v>
+      </c>
+      <c r="C16" s="66" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" s="30" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="30" t="s">
+        <v>416</v>
+      </c>
+      <c r="C17" s="68"/>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B18" t="s">
+        <v>398</v>
+      </c>
+      <c r="C18" s="69">
+        <v>43121</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B19" t="s">
+        <v>397</v>
+      </c>
+      <c r="C19" s="70">
+        <v>7.1527777777777787E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B20" t="s">
+        <v>399</v>
+      </c>
+      <c r="C20" s="66" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B21" t="s">
+        <v>385</v>
+      </c>
+      <c r="C21" s="66" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B22" t="s">
+        <v>400</v>
+      </c>
+      <c r="C22" s="66" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B23" t="s">
+        <v>440</v>
+      </c>
+      <c r="C23" s="66">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B24" t="s">
+        <v>402</v>
+      </c>
+      <c r="C24" s="66" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B25" t="s">
+        <v>404</v>
+      </c>
+      <c r="C25" s="66" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B26" t="s">
+        <v>405</v>
+      </c>
+      <c r="C26" s="66" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B27" t="s">
+        <v>403</v>
+      </c>
+      <c r="C27" s="66" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B28" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" s="30" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B29" s="30" t="s">
+        <v>417</v>
+      </c>
+      <c r="C29" s="68"/>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B30" t="s">
+        <v>398</v>
+      </c>
+      <c r="C30" s="69">
+        <v>43415</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B31" t="s">
+        <v>397</v>
+      </c>
+      <c r="C31" s="70">
+        <v>0.15972222222222224</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B32" t="s">
+        <v>399</v>
+      </c>
+      <c r="C32" s="66" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B33" t="s">
+        <v>385</v>
+      </c>
+      <c r="C33" s="66" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B34" t="s">
+        <v>400</v>
+      </c>
+      <c r="C34" s="66" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B35" t="s">
+        <v>440</v>
+      </c>
+      <c r="C35" s="66">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B36" t="s">
+        <v>402</v>
+      </c>
+      <c r="C36" s="66" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B37" t="s">
+        <v>404</v>
+      </c>
+      <c r="C37" s="66" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B38" t="s">
+        <v>405</v>
+      </c>
+      <c r="C38" s="66" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B39" t="s">
+        <v>403</v>
+      </c>
+      <c r="C39" s="66" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B40" t="s">
+        <v>424</v>
+      </c>
+      <c r="C40" s="66" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3" s="30" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B41" s="30" t="s">
+        <v>418</v>
+      </c>
+      <c r="C41" s="68"/>
+    </row>
+    <row r="42" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B42" t="s">
+        <v>398</v>
+      </c>
+      <c r="C42" s="69">
+        <v>43450</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B43" t="s">
+        <v>397</v>
+      </c>
+      <c r="C43" s="70">
+        <v>0.27291666666666664</v>
+      </c>
+    </row>
+    <row r="44" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B44" t="s">
+        <v>399</v>
+      </c>
+      <c r="C44" s="66" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B45" t="s">
+        <v>385</v>
+      </c>
+      <c r="C45" s="66" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B46" t="s">
+        <v>400</v>
+      </c>
+      <c r="C46" s="66" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B47" t="s">
+        <v>440</v>
+      </c>
+      <c r="C47" s="66">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="48" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B48" t="s">
+        <v>402</v>
+      </c>
+      <c r="C48" s="66" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B49" t="s">
+        <v>404</v>
+      </c>
+      <c r="C49" s="66" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B50" t="s">
+        <v>405</v>
+      </c>
+      <c r="C50" s="66" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B51" t="s">
+        <v>403</v>
+      </c>
+      <c r="C51" s="66" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B52" t="s">
+        <v>424</v>
+      </c>
+      <c r="C52" s="66" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3" s="30" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B53" s="30" t="s">
+        <v>433</v>
+      </c>
+      <c r="C53" s="68"/>
+    </row>
+    <row r="54" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B54" t="s">
+        <v>398</v>
+      </c>
+      <c r="C54" s="69">
+        <v>43552</v>
+      </c>
+    </row>
+    <row r="55" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B55" t="s">
+        <v>397</v>
+      </c>
+      <c r="C55" s="70">
+        <v>0.9770833333333333</v>
+      </c>
+    </row>
+    <row r="56" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B56" t="s">
+        <v>399</v>
+      </c>
+      <c r="C56" s="66" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="57" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B57" t="s">
+        <v>385</v>
+      </c>
+      <c r="C57" s="66" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="58" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B58" t="s">
+        <v>400</v>
+      </c>
+      <c r="C58" s="66" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="59" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B59" t="s">
+        <v>440</v>
+      </c>
+      <c r="C59" s="66">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="60" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B60" t="s">
+        <v>402</v>
+      </c>
+      <c r="C60" s="66" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="61" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B61" t="s">
+        <v>404</v>
+      </c>
+      <c r="C61" s="66" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="62" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B62" t="s">
+        <v>405</v>
+      </c>
+      <c r="C62" s="66" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B63" t="s">
+        <v>403</v>
+      </c>
+      <c r="C63" s="66" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="64" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B64" t="s">
+        <v>424</v>
+      </c>
+      <c r="C64" s="66" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="65" spans="2:3" s="30" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B65" s="30" t="s">
+        <v>435</v>
+      </c>
+      <c r="C65" s="68"/>
+    </row>
+    <row r="66" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B66" t="s">
+        <v>398</v>
+      </c>
+      <c r="C66" s="69">
+        <v>43590</v>
+      </c>
+    </row>
+    <row r="67" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B67" t="s">
+        <v>397</v>
+      </c>
+      <c r="C67" s="70">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="68" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B68" t="s">
+        <v>399</v>
+      </c>
+      <c r="C68" s="66" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="69" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B69" t="s">
+        <v>385</v>
+      </c>
+      <c r="C69" s="66" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="70" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B70" t="s">
+        <v>400</v>
+      </c>
+      <c r="C70" s="66" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="71" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B71" t="s">
+        <v>440</v>
+      </c>
+      <c r="C71" s="66">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="72" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B72" t="s">
+        <v>402</v>
+      </c>
+      <c r="C72" s="66" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="73" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B73" t="s">
+        <v>404</v>
+      </c>
+      <c r="C73" s="66" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="74" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B74" t="s">
+        <v>405</v>
+      </c>
+      <c r="C74" s="66" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B75" t="s">
+        <v>403</v>
+      </c>
+      <c r="C75" s="66" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="76" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B76" t="s">
+        <v>424</v>
+      </c>
+      <c r="C76" s="66" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="77" spans="2:3" s="30" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B77" s="30" t="s">
+        <v>442</v>
+      </c>
+      <c r="C77" s="68"/>
+    </row>
+    <row r="78" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B78" t="s">
+        <v>398</v>
+      </c>
+      <c r="C78" s="69">
+        <v>43645</v>
+      </c>
+    </row>
+    <row r="79" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B79" t="s">
+        <v>397</v>
+      </c>
+      <c r="C79" s="70">
+        <v>0.1875</v>
+      </c>
+    </row>
+    <row r="80" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B80" t="s">
+        <v>399</v>
+      </c>
+      <c r="C80" s="66" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="81" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B81" t="s">
+        <v>385</v>
+      </c>
+      <c r="C81" s="66" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="82" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B82" t="s">
+        <v>400</v>
+      </c>
+      <c r="C82" s="66" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="83" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B83" t="s">
+        <v>402</v>
+      </c>
+      <c r="C83" s="66" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="84" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B84" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="85" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B85" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="86" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B86" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="87" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B87" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="88" spans="2:3" s="30" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C88" s="68"/>
+    </row>
+    <row r="89" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B89" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="90" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B90" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="91" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B91" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="92" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B92" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="93" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B93" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="94" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B94" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="95" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B95" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="96" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B96" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="97" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B97" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="98" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B98" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="99" spans="2:3" s="30" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C99" s="68"/>
+    </row>
+    <row r="100" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B100" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="101" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B101" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="102" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B102" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="103" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B103" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="104" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B104" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="105" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B105" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="106" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B106" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="107" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B107" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="108" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B108" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="109" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B109" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="110" spans="2:3" s="30" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C110" s="68"/>
+    </row>
+    <row r="111" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B111" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="112" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B112" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="113" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B113" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="114" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B114" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="115" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B115" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="116" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B116" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="117" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B117" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="118" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B118" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="119" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B119" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="120" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B120" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="121" spans="2:3" s="30" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C121" s="68"/>
+    </row>
+    <row r="122" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B122" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="123" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B123" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="124" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B124" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="125" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B125" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="126" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B126" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="127" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B127" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="128" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B128" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="129" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B129" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="130" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B130" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="131" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B131" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="135" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A135" t="s">
+        <v>406</v>
+      </c>
+      <c r="B135" s="5">
+        <v>42880</v>
+      </c>
+      <c r="C135" s="70">
+        <v>0.18055555555555555</v>
+      </c>
+      <c r="D135" t="s">
+        <v>342</v>
+      </c>
+      <c r="E135" s="5" t="s">
+        <v>419</v>
+      </c>
+      <c r="F135" t="s">
+        <v>407</v>
+      </c>
+      <c r="G135">
+        <v>0</v>
+      </c>
+      <c r="H135" t="s">
+        <v>408</v>
+      </c>
+      <c r="I135" t="s">
+        <v>413</v>
+      </c>
+      <c r="J135" t="b">
+        <v>0</v>
+      </c>
+      <c r="K135">
+        <v>1</v>
+      </c>
+      <c r="L135" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="136" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A136" t="s">
+        <v>416</v>
+      </c>
+      <c r="B136" s="5">
+        <v>43121</v>
+      </c>
+      <c r="C136" s="70">
+        <v>7.1527777777777787E-2</v>
+      </c>
+      <c r="D136" t="s">
+        <v>342</v>
+      </c>
+      <c r="E136" s="5" t="s">
+        <v>419</v>
+      </c>
+      <c r="F136" t="s">
+        <v>420</v>
+      </c>
+      <c r="G136">
+        <v>13</v>
+      </c>
+      <c r="H136" t="s">
+        <v>409</v>
+      </c>
+      <c r="I136" t="s">
+        <v>414</v>
+      </c>
+      <c r="J136" t="b">
+        <v>0</v>
+      </c>
+      <c r="K136">
+        <v>2</v>
+      </c>
+      <c r="L136" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="137" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A137" t="s">
+        <v>417</v>
+      </c>
+      <c r="B137" s="5">
+        <v>43415</v>
+      </c>
+      <c r="C137" s="70">
+        <v>0.15972222222222224</v>
+      </c>
+      <c r="D137" t="s">
+        <v>342</v>
+      </c>
+      <c r="E137" s="5" t="s">
+        <v>419</v>
+      </c>
+      <c r="F137" t="s">
+        <v>421</v>
+      </c>
+      <c r="G137">
+        <v>45</v>
+      </c>
+      <c r="H137" t="s">
+        <v>408</v>
+      </c>
+      <c r="I137" t="s">
+        <v>414</v>
+      </c>
+      <c r="J137" t="b">
+        <v>0</v>
+      </c>
+      <c r="K137">
+        <v>4</v>
+      </c>
+      <c r="L137" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="138" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A138" t="s">
+        <v>418</v>
+      </c>
+      <c r="B138" s="5">
+        <v>43450</v>
+      </c>
+      <c r="C138" s="70">
+        <v>0.27291666666666664</v>
+      </c>
+      <c r="D138" t="s">
+        <v>342</v>
+      </c>
+      <c r="E138" s="5" t="s">
+        <v>419</v>
+      </c>
+      <c r="F138" t="s">
+        <v>422</v>
+      </c>
+      <c r="G138">
+        <v>78</v>
+      </c>
+      <c r="H138" t="s">
+        <v>408</v>
+      </c>
+      <c r="I138" t="s">
+        <v>414</v>
+      </c>
+      <c r="J138" t="b">
+        <v>0</v>
+      </c>
+      <c r="K138">
+        <v>1</v>
+      </c>
+      <c r="L138" t="s">
+        <v>423</v>
+      </c>
+      <c r="M138" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="139" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="D139" t="s">
+        <v>342</v>
+      </c>
+      <c r="E139" s="5"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" display="Launches" xr:uid="{150C44E6-114D-433C-B6DD-97B7D35EAC74}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R25"/>
   <sheetViews>
@@ -13116,7 +14248,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B31"/>
   <sheetViews>
@@ -13372,7 +14504,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B40"/>
   <sheetViews>
@@ -13702,7 +14834,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B29"/>
   <sheetViews>

</xml_diff>